<commit_message>
logo added of gemini
</commit_message>
<xml_diff>
--- a/public/changes.xlsx
+++ b/public/changes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Website changes</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Post a question and review to be added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git </t>
   </si>
   <si>
     <t>Let AI write for me along with virtual tryon</t>
@@ -1186,8 +1189,8 @@
   <sheetPr/>
   <dimension ref="A5:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -1511,7 +1514,7 @@
       <c r="A45">
         <v>5</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1554,7 +1557,9 @@
       <c r="B51" s="5"/>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="5"/>
+      <c r="B52" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="5"/>
@@ -1576,25 +1581,25 @@
     </row>
     <row r="60" spans="2:2">
       <c r="B60" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1602,12 +1607,12 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error for place your rental
</commit_message>
<xml_diff>
--- a/public/changes.xlsx
+++ b/public/changes.xlsx
@@ -1190,7 +1190,7 @@
   <dimension ref="A5:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -1482,7 +1482,7 @@
       <c r="A41">
         <v>1</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>